<commit_message>
SP Sunday May 3 1:27 pm commit
</commit_message>
<xml_diff>
--- a/wp3/Ranks.xlsx
+++ b/wp3/Ranks.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t xml:space="preserve">en_rgnames</t>
   </si>
@@ -96,12 +96,6 @@
   </si>
   <si>
     <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nenetskiy Aok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
   </si>
   <si>
     <t xml:space="preserve">Belgorodskaya Oblast</t>
@@ -893,16 +887,16 @@
         <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" t="n">
-        <v>44.5</v>
+        <v>43.5</v>
       </c>
       <c r="E2" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -925,16 +919,16 @@
         <v>13</v>
       </c>
       <c r="C3" t="n">
-        <v>15.5</v>
+        <v>14.5</v>
       </c>
       <c r="D3" t="n">
-        <v>33.5</v>
+        <v>32.5</v>
       </c>
       <c r="E3" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -957,16 +951,16 @@
         <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>39.5</v>
+        <v>39</v>
       </c>
       <c r="D4" t="n">
         <v>9</v>
       </c>
       <c r="E4" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -989,16 +983,16 @@
         <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>51.25</v>
+        <v>50.25</v>
       </c>
       <c r="D5" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -1021,16 +1015,16 @@
         <v>19</v>
       </c>
       <c r="C6" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1053,16 +1047,16 @@
         <v>21</v>
       </c>
       <c r="C7" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -1085,16 +1079,16 @@
         <v>23</v>
       </c>
       <c r="C8" t="n">
-        <v>63.5</v>
+        <v>62.5</v>
       </c>
       <c r="D8" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -1117,16 +1111,16 @@
         <v>25</v>
       </c>
       <c r="C9" t="n">
-        <v>24.75</v>
+        <v>24</v>
       </c>
       <c r="D9" t="n">
-        <v>12.5</v>
+        <v>12</v>
       </c>
       <c r="E9" t="n">
         <v>4</v>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -1149,10 +1143,10 @@
         <v>27</v>
       </c>
       <c r="C10" t="n">
-        <v>44.5</v>
+        <v>43.5</v>
       </c>
       <c r="D10" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" t="n">
         <v>2</v>
@@ -1181,19 +1175,19 @@
         <v>29</v>
       </c>
       <c r="C11" t="n">
-        <v>11.25</v>
+        <v>39</v>
       </c>
       <c r="D11" t="n">
-        <v>12.5</v>
+        <v>4</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1202,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -1213,16 +1207,16 @@
         <v>31</v>
       </c>
       <c r="C12" t="n">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E12" t="n">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F12" t="n">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -1245,16 +1239,16 @@
         <v>33</v>
       </c>
       <c r="C13" t="n">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D13" t="n">
-        <v>19</v>
+        <v>32.5</v>
       </c>
       <c r="E13" t="n">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="F13" t="n">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -1277,28 +1271,28 @@
         <v>35</v>
       </c>
       <c r="C14" t="n">
-        <v>43</v>
+        <v>50.5</v>
       </c>
       <c r="D14" t="n">
-        <v>33.5</v>
+        <v>24</v>
       </c>
       <c r="E14" t="n">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="F14" t="n">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1309,16 +1303,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>51.5</v>
+        <v>60</v>
       </c>
       <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="n">
+        <v>9</v>
+      </c>
+      <c r="F15" t="n">
         <v>25</v>
-      </c>
-      <c r="E15" t="n">
-        <v>22</v>
-      </c>
-      <c r="F15" t="n">
-        <v>11</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -1341,25 +1335,25 @@
         <v>39</v>
       </c>
       <c r="C16" t="n">
-        <v>61</v>
+        <v>22.5</v>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="F16" t="n">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1373,16 +1367,16 @@
         <v>41</v>
       </c>
       <c r="C17" t="n">
-        <v>23.5</v>
+        <v>42</v>
       </c>
       <c r="D17" t="n">
-        <v>52</v>
+        <v>37.5</v>
       </c>
       <c r="E17" t="n">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F17" t="n">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -1391,10 +1385,10 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1405,16 +1399,16 @@
         <v>43</v>
       </c>
       <c r="C18" t="n">
-        <v>43</v>
+        <v>37.5</v>
       </c>
       <c r="D18" t="n">
-        <v>38.5</v>
+        <v>65.5</v>
       </c>
       <c r="E18" t="n">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="F18" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1423,10 +1417,10 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1437,25 +1431,25 @@
         <v>45</v>
       </c>
       <c r="C19" t="n">
-        <v>38.5</v>
+        <v>41</v>
       </c>
       <c r="D19" t="n">
-        <v>66.5</v>
+        <v>16</v>
       </c>
       <c r="E19" t="n">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="F19" t="n">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -1469,25 +1463,25 @@
         <v>47</v>
       </c>
       <c r="C20" t="n">
-        <v>42</v>
+        <v>23.75</v>
       </c>
       <c r="D20" t="n">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="E20" t="n">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="F20" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
@@ -1501,16 +1495,16 @@
         <v>49</v>
       </c>
       <c r="C21" t="n">
-        <v>24.25</v>
+        <v>24.5</v>
       </c>
       <c r="D21" t="n">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="E21" t="n">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F21" t="n">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -1533,16 +1527,16 @@
         <v>51</v>
       </c>
       <c r="C22" t="n">
-        <v>25.5</v>
+        <v>53</v>
       </c>
       <c r="D22" t="n">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="E22" t="n">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F22" t="n">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
@@ -1565,16 +1559,16 @@
         <v>53</v>
       </c>
       <c r="C23" t="n">
-        <v>54</v>
+        <v>26.5</v>
       </c>
       <c r="D23" t="n">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="E23" t="n">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F23" t="n">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1597,16 +1591,16 @@
         <v>55</v>
       </c>
       <c r="C24" t="n">
-        <v>27</v>
+        <v>39.5</v>
       </c>
       <c r="D24" t="n">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="E24" t="n">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="F24" t="n">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1629,16 +1623,16 @@
         <v>57</v>
       </c>
       <c r="C25" t="n">
-        <v>40</v>
+        <v>48.5</v>
       </c>
       <c r="D25" t="n">
-        <v>73</v>
+        <v>19.5</v>
       </c>
       <c r="E25" t="n">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="F25" t="n">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
@@ -1647,10 +1641,10 @@
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1661,16 +1655,16 @@
         <v>59</v>
       </c>
       <c r="C26" t="n">
-        <v>49.5</v>
+        <v>68</v>
       </c>
       <c r="D26" t="n">
-        <v>20.5</v>
+        <v>42</v>
       </c>
       <c r="E26" t="n">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F26" t="n">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
@@ -1696,25 +1690,25 @@
         <v>69</v>
       </c>
       <c r="D27" t="n">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="E27" t="n">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="F27" t="n">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1725,28 +1719,28 @@
         <v>63</v>
       </c>
       <c r="C28" t="n">
-        <v>70</v>
+        <v>14.5</v>
       </c>
       <c r="D28" t="n">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="E28" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F28" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1757,16 +1751,16 @@
         <v>65</v>
       </c>
       <c r="C29" t="n">
-        <v>15.5</v>
+        <v>72</v>
       </c>
       <c r="D29" t="n">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="E29" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F29" t="n">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -1789,25 +1783,25 @@
         <v>67</v>
       </c>
       <c r="C30" t="n">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="D30" t="n">
-        <v>49</v>
+        <v>37.5</v>
       </c>
       <c r="E30" t="n">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F30" t="n">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -1821,16 +1815,16 @@
         <v>69</v>
       </c>
       <c r="C31" t="n">
-        <v>27</v>
+        <v>2.5</v>
       </c>
       <c r="D31" t="n">
-        <v>38.5</v>
+        <v>65.5</v>
       </c>
       <c r="E31" t="n">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="F31" t="n">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -1853,16 +1847,16 @@
         <v>71</v>
       </c>
       <c r="C32" t="n">
-        <v>2.5</v>
+        <v>9.5</v>
       </c>
       <c r="D32" t="n">
-        <v>66.5</v>
+        <v>19.5</v>
       </c>
       <c r="E32" t="n">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="F32" t="n">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -1885,25 +1879,25 @@
         <v>73</v>
       </c>
       <c r="C33" t="n">
-        <v>10</v>
+        <v>47.5</v>
       </c>
       <c r="D33" t="n">
-        <v>20.5</v>
+        <v>8</v>
       </c>
       <c r="E33" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F33" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="n">
         <v>0</v>
@@ -1917,25 +1911,25 @@
         <v>75</v>
       </c>
       <c r="C34" t="n">
-        <v>48.5</v>
+        <v>48</v>
       </c>
       <c r="D34" t="n">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="E34" t="n">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="F34" t="n">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="n">
         <v>0</v>
@@ -1949,16 +1943,16 @@
         <v>77</v>
       </c>
       <c r="C35" t="n">
-        <v>49</v>
+        <v>1.5</v>
       </c>
       <c r="D35" t="n">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E35" t="n">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="F35" t="n">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
@@ -1981,16 +1975,16 @@
         <v>79</v>
       </c>
       <c r="C36" t="n">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="D36" t="n">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E36" t="n">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="F36" t="n">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
@@ -2013,25 +2007,25 @@
         <v>81</v>
       </c>
       <c r="C37" t="n">
-        <v>3.5</v>
+        <v>46</v>
       </c>
       <c r="D37" t="n">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E37" t="n">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="F37" t="n">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
         <v>0</v>
@@ -2045,19 +2039,19 @@
         <v>83</v>
       </c>
       <c r="C38" t="n">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D38" t="n">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="E38" t="n">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="F38" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -2066,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -2077,19 +2071,19 @@
         <v>85</v>
       </c>
       <c r="C39" t="n">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="D39" t="n">
-        <v>24</v>
+        <v>67.5</v>
       </c>
       <c r="E39" t="n">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="F39" t="n">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -2098,7 +2092,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2109,19 +2103,19 @@
         <v>87</v>
       </c>
       <c r="C40" t="n">
-        <v>26.5</v>
+        <v>55.5</v>
       </c>
       <c r="D40" t="n">
-        <v>68.5</v>
+        <v>10</v>
       </c>
       <c r="E40" t="n">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="F40" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="G40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -2130,7 +2124,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -2141,16 +2135,16 @@
         <v>89</v>
       </c>
       <c r="C41" t="n">
-        <v>56.5</v>
+        <v>23</v>
       </c>
       <c r="D41" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E41" t="n">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="F41" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G41" t="n">
         <v>0</v>
@@ -2173,16 +2167,16 @@
         <v>91</v>
       </c>
       <c r="C42" t="n">
-        <v>23.5</v>
+        <v>48.5</v>
       </c>
       <c r="D42" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E42" t="n">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="F42" t="n">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="G42" t="n">
         <v>0</v>
@@ -2205,16 +2199,16 @@
         <v>93</v>
       </c>
       <c r="C43" t="n">
-        <v>49.5</v>
+        <v>53.5</v>
       </c>
       <c r="D43" t="n">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E43" t="n">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="F43" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
@@ -2223,10 +2217,10 @@
         <v>0</v>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -2237,16 +2231,16 @@
         <v>95</v>
       </c>
       <c r="C44" t="n">
-        <v>54.5</v>
+        <v>33.5</v>
       </c>
       <c r="D44" t="n">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="F44" t="n">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
@@ -2255,10 +2249,10 @@
         <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -2269,16 +2263,16 @@
         <v>97</v>
       </c>
       <c r="C45" t="n">
-        <v>34</v>
+        <v>59.5</v>
       </c>
       <c r="D45" t="n">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="E45" t="n">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="F45" t="n">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
@@ -2301,19 +2295,19 @@
         <v>99</v>
       </c>
       <c r="C46" t="n">
-        <v>60.5</v>
+        <v>18</v>
       </c>
       <c r="D46" t="n">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="E46" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F46" t="n">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -2322,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2333,19 +2327,19 @@
         <v>101</v>
       </c>
       <c r="C47" t="n">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="D47" t="n">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E47" t="n">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F47" t="n">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="G47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -2354,7 +2348,7 @@
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -2365,16 +2359,16 @@
         <v>103</v>
       </c>
       <c r="C48" t="n">
-        <v>45</v>
+        <v>36.5</v>
       </c>
       <c r="D48" t="n">
-        <v>17</v>
+        <v>43.5</v>
       </c>
       <c r="E48" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F48" t="n">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="G48" t="n">
         <v>0</v>
@@ -2383,10 +2377,10 @@
         <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -2397,25 +2391,25 @@
         <v>105</v>
       </c>
       <c r="C49" t="n">
-        <v>37.5</v>
+        <v>48.5</v>
       </c>
       <c r="D49" t="n">
-        <v>44.5</v>
+        <v>27</v>
       </c>
       <c r="E49" t="n">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="F49" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G49" t="n">
         <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="n">
         <v>0</v>
@@ -2429,16 +2423,16 @@
         <v>107</v>
       </c>
       <c r="C50" t="n">
-        <v>49.5</v>
+        <v>30.5</v>
       </c>
       <c r="D50" t="n">
         <v>28</v>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F50" t="n">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="G50" t="n">
         <v>0</v>
@@ -2461,28 +2455,28 @@
         <v>109</v>
       </c>
       <c r="C51" t="n">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D51" t="n">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E51" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F51" t="n">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="G51" t="n">
         <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -2493,16 +2487,16 @@
         <v>111</v>
       </c>
       <c r="C52" t="n">
-        <v>42</v>
+        <v>63.5</v>
       </c>
       <c r="D52" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E52" t="n">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="F52" t="n">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="G52" t="n">
         <v>0</v>
@@ -2525,19 +2519,19 @@
         <v>113</v>
       </c>
       <c r="C53" t="n">
-        <v>64.5</v>
+        <v>10</v>
       </c>
       <c r="D53" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E53" t="n">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="F53" t="n">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -2546,7 +2540,7 @@
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2557,19 +2551,19 @@
         <v>115</v>
       </c>
       <c r="C54" t="n">
-        <v>10.5</v>
+        <v>48</v>
       </c>
       <c r="D54" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="F54" t="n">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -2578,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="J54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -2589,19 +2583,19 @@
         <v>117</v>
       </c>
       <c r="C55" t="n">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D55" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E55" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -2610,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="J55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2621,22 +2615,22 @@
         <v>119</v>
       </c>
       <c r="C56" t="n">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
       <c r="D56" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
@@ -2653,25 +2647,25 @@
         <v>121</v>
       </c>
       <c r="C57" t="n">
-        <v>22.5</v>
+        <v>39.5</v>
       </c>
       <c r="D57" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E57" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F57" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G57" t="n">
         <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J57" t="n">
         <v>0</v>
@@ -2685,16 +2679,16 @@
         <v>123</v>
       </c>
       <c r="C58" t="n">
-        <v>40.5</v>
+        <v>33.5</v>
       </c>
       <c r="D58" t="n">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="E58" t="n">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F58" t="n">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="G58" t="n">
         <v>0</v>
@@ -2703,10 +2697,10 @@
         <v>0</v>
       </c>
       <c r="I58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -2717,19 +2711,19 @@
         <v>125</v>
       </c>
       <c r="C59" t="n">
-        <v>34.5</v>
+        <v>59.25</v>
       </c>
       <c r="D59" t="n">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="E59" t="n">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="G59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -2738,7 +2732,7 @@
         <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2749,22 +2743,22 @@
         <v>127</v>
       </c>
       <c r="C60" t="n">
-        <v>60.25</v>
+        <v>50.5</v>
       </c>
       <c r="D60" t="n">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="E60" t="n">
         <v>11</v>
       </c>
       <c r="F60" t="n">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" t="n">
         <v>0</v>
@@ -2781,25 +2775,25 @@
         <v>129</v>
       </c>
       <c r="C61" t="n">
-        <v>51.5</v>
+        <v>48.5</v>
       </c>
       <c r="D61" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E61" t="n">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="F61" t="n">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="G61" t="n">
         <v>0</v>
       </c>
       <c r="H61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" t="n">
         <v>0</v>
@@ -2813,25 +2807,25 @@
         <v>131</v>
       </c>
       <c r="C62" t="n">
-        <v>49.5</v>
+        <v>33</v>
       </c>
       <c r="D62" t="n">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="E62" t="n">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="F62" t="n">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="G62" t="n">
         <v>0</v>
       </c>
       <c r="H62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62" t="n">
         <v>0</v>
@@ -2845,25 +2839,25 @@
         <v>133</v>
       </c>
       <c r="C63" t="n">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D63" t="n">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="E63" t="n">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="F63" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="G63" t="n">
         <v>0</v>
       </c>
       <c r="H63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" t="n">
         <v>0</v>
@@ -2877,16 +2871,16 @@
         <v>135</v>
       </c>
       <c r="C64" t="n">
-        <v>56</v>
+        <v>43.5</v>
       </c>
       <c r="D64" t="n">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E64" t="n">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="F64" t="n">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="G64" t="n">
         <v>0</v>
@@ -2895,10 +2889,10 @@
         <v>0</v>
       </c>
       <c r="I64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -2909,16 +2903,16 @@
         <v>137</v>
       </c>
       <c r="C65" t="n">
-        <v>44.5</v>
+        <v>30.5</v>
       </c>
       <c r="D65" t="n">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="E65" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F65" t="n">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="G65" t="n">
         <v>0</v>
@@ -2927,10 +2921,10 @@
         <v>0</v>
       </c>
       <c r="I65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2941,25 +2935,25 @@
         <v>139</v>
       </c>
       <c r="C66" t="n">
-        <v>31.5</v>
+        <v>56.25</v>
       </c>
       <c r="D66" t="n">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="E66" t="n">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="F66" t="n">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="G66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
       </c>
       <c r="I66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J66" t="n">
         <v>0</v>
@@ -2973,25 +2967,25 @@
         <v>141</v>
       </c>
       <c r="C67" t="n">
-        <v>57.25</v>
+        <v>48</v>
       </c>
       <c r="D67" t="n">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="F67" t="n">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="G67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
       </c>
       <c r="I67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J67" t="n">
         <v>0</v>
@@ -3005,25 +2999,25 @@
         <v>143</v>
       </c>
       <c r="C68" t="n">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D68" t="n">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E68" t="n">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="F68" t="n">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="G68" t="n">
         <v>0</v>
       </c>
       <c r="H68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" t="n">
         <v>0</v>
@@ -3037,28 +3031,28 @@
         <v>145</v>
       </c>
       <c r="C69" t="n">
-        <v>60</v>
+        <v>50.5</v>
       </c>
       <c r="D69" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E69" t="n">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="F69" t="n">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="G69" t="n">
         <v>0</v>
       </c>
       <c r="H69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" t="n">
         <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -3069,16 +3063,16 @@
         <v>147</v>
       </c>
       <c r="C70" t="n">
-        <v>51.5</v>
+        <v>30</v>
       </c>
       <c r="D70" t="n">
-        <v>36</v>
+        <v>67.5</v>
       </c>
       <c r="E70" t="n">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="F70" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G70" t="n">
         <v>0</v>
@@ -3087,10 +3081,10 @@
         <v>0</v>
       </c>
       <c r="I70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -3101,16 +3095,16 @@
         <v>149</v>
       </c>
       <c r="C71" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D71" t="n">
-        <v>68.5</v>
+        <v>70</v>
       </c>
       <c r="E71" t="n">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F71" t="n">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="G71" t="n">
         <v>0</v>
@@ -3133,16 +3127,16 @@
         <v>151</v>
       </c>
       <c r="C72" t="n">
-        <v>36.5</v>
+        <v>46</v>
       </c>
       <c r="D72" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E72" t="n">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F72" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G72" t="n">
         <v>0</v>
@@ -3165,16 +3159,16 @@
         <v>153</v>
       </c>
       <c r="C73" t="n">
-        <v>47</v>
+        <v>20.5</v>
       </c>
       <c r="D73" t="n">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="E73" t="n">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="F73" t="n">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="G73" t="n">
         <v>0</v>
@@ -3183,10 +3177,10 @@
         <v>0</v>
       </c>
       <c r="I73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -3197,19 +3191,19 @@
         <v>155</v>
       </c>
       <c r="C74" t="n">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="D74" t="n">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="E74" t="n">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F74" t="n">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -3218,7 +3212,7 @@
         <v>0</v>
       </c>
       <c r="J74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -3229,19 +3223,19 @@
         <v>157</v>
       </c>
       <c r="C75" t="n">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D75" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="F75" t="n">
         <v>68</v>
       </c>
       <c r="G75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -3250,7 +3244,7 @@
         <v>0</v>
       </c>
       <c r="J75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -3261,19 +3255,19 @@
         <v>159</v>
       </c>
       <c r="C76" t="n">
-        <v>31</v>
+        <v>57.5</v>
       </c>
       <c r="D76" t="n">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="E76" t="n">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="F76" t="n">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="G76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -3282,7 +3276,7 @@
         <v>0</v>
       </c>
       <c r="J76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -3293,25 +3287,25 @@
         <v>161</v>
       </c>
       <c r="C77" t="n">
-        <v>58.5</v>
+        <v>41.5</v>
       </c>
       <c r="D77" t="n">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="E77" t="n">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="F77" t="n">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
       </c>
       <c r="I77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J77" t="n">
         <v>0</v>
@@ -3325,16 +3319,16 @@
         <v>163</v>
       </c>
       <c r="C78" t="n">
-        <v>42</v>
+        <v>50.5</v>
       </c>
       <c r="D78" t="n">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="E78" t="n">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="F78" t="n">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="G78" t="n">
         <v>0</v>
@@ -3357,16 +3351,16 @@
         <v>165</v>
       </c>
       <c r="C79" t="n">
-        <v>51.5</v>
+        <v>38.5</v>
       </c>
       <c r="D79" t="n">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="E79" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F79" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G79" t="n">
         <v>0</v>
@@ -3375,10 +3369,10 @@
         <v>0</v>
       </c>
       <c r="I79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -3389,19 +3383,19 @@
         <v>167</v>
       </c>
       <c r="C80" t="n">
-        <v>39.5</v>
+        <v>74.5</v>
       </c>
       <c r="D80" t="n">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="E80" t="n">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F80" t="n">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -3410,38 +3404,6 @@
         <v>0</v>
       </c>
       <c r="J80" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s">
-        <v>168</v>
-      </c>
-      <c r="B81" t="s">
-        <v>169</v>
-      </c>
-      <c r="C81" t="n">
-        <v>75.5</v>
-      </c>
-      <c r="D81" t="n">
-        <v>76</v>
-      </c>
-      <c r="E81" t="n">
-        <v>25</v>
-      </c>
-      <c r="F81" t="n">
-        <v>32</v>
-      </c>
-      <c r="G81" t="n">
-        <v>1</v>
-      </c>
-      <c r="H81" t="n">
-        <v>0</v>
-      </c>
-      <c r="I81" t="n">
-        <v>0</v>
-      </c>
-      <c r="J81" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>